<commit_message>
Aula 4 - Manipulando Arquivos | Curso em Vídeo ✅
E corrigi algumas coisas que tive na ultima aula da FATEC.
Programação em Microinformática.
</commit_message>
<xml_diff>
--- a/[02]-exercicios-fatec/EXERCICIO ESTOQUE.xlsx
+++ b/[02]-exercicios-fatec/EXERCICIO ESTOQUE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\Programação em Microinformática\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duanl\Documents\FATEC\Programação em Microinformática\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E99DFE-2CD6-4FA0-83DC-5EB3A40D3CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB33619-A091-4522-B4DF-909DC3D74B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Estoque" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
     <sheet name="Vendas do Mes" sheetId="3" r:id="rId3"/>
     <sheet name="Restante do Estoque" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -363,7 +376,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -431,6 +444,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -446,7 +466,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -623,57 +643,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="double">
-        <color indexed="12"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="12"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color indexed="12"/>
       </left>
@@ -718,10 +687,41 @@
     <border>
       <left/>
       <right style="double">
-        <color rgb="FF002060"/>
+        <color rgb="FF0000FF"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF0000FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color rgb="FF0000FF"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF0000FF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color rgb="FF0000FF"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -729,7 +729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -764,6 +764,18 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -803,34 +815,29 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -838,6 +845,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF990000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1102,7 +1115,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Restante do Estoque'!$I$29:$I$30</c:f>
+              <c:f>'Restante do Estoque'!$I$34:$I$35</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1116,7 +1129,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Restante do Estoque'!$J$29:$J$30</c:f>
+              <c:f>'Restante do Estoque'!$J$34:$J$35</c:f>
               <c:numCache>
                 <c:formatCode>_("R$ "* #,##0.00_);_("R$ "* \(#,##0.00\);_("R$ "* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1801,8 +1814,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1831,9 +1844,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1871,9 +1884,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1906,26 +1919,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1958,26 +1954,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2153,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showZeros="0" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2171,7 +2150,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickTop="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>36</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -2184,12 +2163,12 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="29"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="14"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:9" ht="13.5" thickBot="1">
-      <c r="A3" s="29"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="15" t="s">
         <v>34</v>
       </c>
@@ -2200,14 +2179,14 @@
       <c r="G3" s="17"/>
     </row>
     <row r="4" spans="1:9" ht="13.5" thickTop="1">
-      <c r="A4" s="29"/>
-      <c r="F4" s="31" t="s">
+      <c r="A4" s="39"/>
+      <c r="F4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="32"/>
+      <c r="G4" s="42"/>
     </row>
     <row r="5" spans="1:9" ht="25.5">
-      <c r="A5" s="29"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2230,7 +2209,7 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="29"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="10">
         <v>39448</v>
       </c>
@@ -2247,13 +2226,13 @@
         <f>IF(D6=1,E6,0)</f>
         <v>0</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="65">
         <f>IF(D6=2,E6,0)</f>
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="29"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="10">
         <v>39448</v>
       </c>
@@ -2270,13 +2249,13 @@
         <f t="shared" ref="F7:F36" si="0">IF(D7=1,E7,0)</f>
         <v>110</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="65">
         <f t="shared" ref="G7:G36" si="1">IF(D7=2,E7,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="29"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="10">
         <v>39448</v>
       </c>
@@ -2293,13 +2272,13 @@
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="66">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="29"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="10">
         <v>39448</v>
       </c>
@@ -2316,13 +2295,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="65">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="29"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="10">
         <v>39448</v>
       </c>
@@ -2339,13 +2318,13 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="29"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="10">
         <v>39448</v>
       </c>
@@ -2362,13 +2341,13 @@
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="29"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="10">
         <v>39448</v>
       </c>
@@ -2385,13 +2364,13 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="G12" s="52">
+      <c r="G12" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="29"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="10">
         <v>39448</v>
       </c>
@@ -2408,13 +2387,13 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="G13" s="52">
+      <c r="G13" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="29"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="10">
         <v>39448</v>
       </c>
@@ -2431,13 +2410,13 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G14" s="52">
+      <c r="G14" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="29"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="10">
         <v>39448</v>
       </c>
@@ -2447,20 +2426,20 @@
       <c r="D15">
         <v>1</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="29">
         <v>50</v>
       </c>
       <c r="F15" s="11">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G15" s="52">
+      <c r="G15" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="29"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="10">
         <v>39448</v>
       </c>
@@ -2477,13 +2456,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G16" s="52">
+      <c r="G16" s="65">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="29"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="10">
         <v>39448</v>
       </c>
@@ -2500,13 +2479,13 @@
         <f t="shared" si="0"/>
         <v>95</v>
       </c>
-      <c r="G17" s="52">
+      <c r="G17" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="29"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="10">
         <v>39448</v>
       </c>
@@ -2523,13 +2502,13 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G18" s="52">
+      <c r="G18" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="29"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="10">
         <v>39448</v>
       </c>
@@ -2546,13 +2525,13 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G19" s="52">
+      <c r="G19" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="29"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="10">
         <v>39448</v>
       </c>
@@ -2569,13 +2548,13 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="G20" s="52">
+      <c r="G20" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="29"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="10">
         <v>39448</v>
       </c>
@@ -2592,13 +2571,13 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G21" s="52">
+      <c r="G21" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="29"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="10">
         <v>39448</v>
       </c>
@@ -2615,13 +2594,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G22" s="52">
+      <c r="G22" s="65">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="29"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="10">
         <v>39448</v>
       </c>
@@ -2638,13 +2617,13 @@
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="G23" s="52">
+      <c r="G23" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="29"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="10">
         <v>39448</v>
       </c>
@@ -2661,13 +2640,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G24" s="52">
+      <c r="G24" s="65">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="29"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="10">
         <v>39448</v>
       </c>
@@ -2684,13 +2663,13 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="G25" s="52">
+      <c r="G25" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="29"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="10">
         <v>39448</v>
       </c>
@@ -2707,13 +2686,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="52">
+      <c r="G26" s="65">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="29"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="10">
         <v>39448</v>
       </c>
@@ -2730,13 +2709,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="52">
+      <c r="G27" s="65">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="29"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="10">
         <v>39448</v>
       </c>
@@ -2753,13 +2732,13 @@
         <f t="shared" si="0"/>
         <v>650</v>
       </c>
-      <c r="G28" s="52">
+      <c r="G28" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="29"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="10">
         <v>39448</v>
       </c>
@@ -2776,13 +2755,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G29" s="52">
+      <c r="G29" s="65">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="29"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="10">
         <v>39448</v>
       </c>
@@ -2799,13 +2778,13 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="G30" s="52">
+      <c r="G30" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="29"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="10">
         <v>39448</v>
       </c>
@@ -2822,13 +2801,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="52">
+      <c r="G31" s="65">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="29"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="10">
         <v>39448</v>
       </c>
@@ -2845,13 +2824,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G32" s="52">
+      <c r="G32" s="65">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="29"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="10">
         <v>39448</v>
       </c>
@@ -2868,13 +2847,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G33" s="52">
+      <c r="G33" s="65">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="29"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="10">
         <v>39448</v>
       </c>
@@ -2891,13 +2870,13 @@
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="G34" s="52">
+      <c r="G34" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="29"/>
+      <c r="A35" s="39"/>
       <c r="B35" s="10">
         <v>39448</v>
       </c>
@@ -2914,30 +2893,30 @@
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="G35" s="52">
+      <c r="G35" s="65">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="13.5" thickBot="1">
-      <c r="A36" s="30"/>
-      <c r="B36" s="46">
-        <v>39448</v>
-      </c>
-      <c r="C36" s="47" t="s">
+      <c r="A36" s="40"/>
+      <c r="B36" s="34">
+        <v>39448</v>
+      </c>
+      <c r="C36" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="47">
+      <c r="D36" s="57">
         <v>2</v>
       </c>
-      <c r="E36" s="47">
+      <c r="E36" s="57">
         <v>50</v>
       </c>
-      <c r="F36" s="48">
+      <c r="F36" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G36" s="53">
+      <c r="G36" s="64">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
@@ -2986,8 +2965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3000,7 +2979,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickTop="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>44</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -3011,12 +2990,12 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="29"/>
+      <c r="A2" s="39"/>
       <c r="B2" s="14"/>
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A3" s="29"/>
+      <c r="A3" s="39"/>
       <c r="B3" s="15" t="s">
         <v>34</v>
       </c>
@@ -3025,11 +3004,11 @@
       <c r="E3" s="17"/>
     </row>
     <row r="4" spans="1:5" ht="13.5" thickTop="1">
-      <c r="A4" s="29"/>
+      <c r="A4" s="39"/>
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="29"/>
+      <c r="A5" s="39"/>
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -3044,7 +3023,7 @@
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="29"/>
+      <c r="A6" s="39"/>
       <c r="B6" s="10">
         <v>39480</v>
       </c>
@@ -3060,7 +3039,7 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="29"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="10">
         <v>39480</v>
       </c>
@@ -3076,7 +3055,7 @@
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="29"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="10">
         <v>39480</v>
       </c>
@@ -3092,7 +3071,7 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="29"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="10">
         <v>39480</v>
       </c>
@@ -3108,7 +3087,7 @@
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="29"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="10">
         <v>39480</v>
       </c>
@@ -3124,7 +3103,7 @@
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="29"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="10">
         <v>39480</v>
       </c>
@@ -3140,7 +3119,7 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="29"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="10">
         <v>39480</v>
       </c>
@@ -3156,7 +3135,7 @@
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="29"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="10">
         <v>39480</v>
       </c>
@@ -3172,7 +3151,7 @@
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="29"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="10">
         <v>39480</v>
       </c>
@@ -3188,7 +3167,7 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="29"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="10">
         <v>39480</v>
       </c>
@@ -3204,7 +3183,7 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="29"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="10">
         <v>39480</v>
       </c>
@@ -3220,7 +3199,7 @@
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="29"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="10">
         <v>39480</v>
       </c>
@@ -3236,7 +3215,7 @@
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="29"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="10">
         <v>39480</v>
       </c>
@@ -3252,7 +3231,7 @@
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="29"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="10">
         <v>39480</v>
       </c>
@@ -3268,7 +3247,7 @@
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="29"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="10">
         <v>39480</v>
       </c>
@@ -3284,7 +3263,7 @@
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="29"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="10">
         <v>39480</v>
       </c>
@@ -3300,7 +3279,7 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="29"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="10">
         <v>39480</v>
       </c>
@@ -3316,7 +3295,7 @@
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="29"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="10">
         <v>39480</v>
       </c>
@@ -3332,7 +3311,7 @@
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="29"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="10">
         <v>39480</v>
       </c>
@@ -3348,7 +3327,7 @@
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="29"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="10">
         <v>39480</v>
       </c>
@@ -3364,7 +3343,7 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="29"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="10">
         <v>39480</v>
       </c>
@@ -3380,7 +3359,7 @@
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="29"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="10">
         <v>39480</v>
       </c>
@@ -3396,7 +3375,7 @@
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="29"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="10">
         <v>39480</v>
       </c>
@@ -3412,7 +3391,7 @@
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="29"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="10">
         <v>39480</v>
       </c>
@@ -3428,7 +3407,7 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="29"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="10">
         <v>39480</v>
       </c>
@@ -3444,11 +3423,11 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="29"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="10">
         <v>39480</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C31" s="67" t="s">
         <v>28</v>
       </c>
       <c r="D31" s="21">
@@ -3460,7 +3439,7 @@
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="29"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="10">
         <v>39480</v>
       </c>
@@ -3476,7 +3455,7 @@
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="29"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="10">
         <v>39480</v>
       </c>
@@ -3492,7 +3471,7 @@
       </c>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="29"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="10">
         <v>39480</v>
       </c>
@@ -3508,7 +3487,7 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="29"/>
+      <c r="A35" s="39"/>
       <c r="B35" s="10">
         <v>39480</v>
       </c>
@@ -3524,37 +3503,37 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A36" s="30"/>
-      <c r="B36" s="46">
+      <c r="A36" s="40"/>
+      <c r="B36" s="34">
         <v>39480</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D36" s="51">
+      <c r="D36" s="62">
         <v>0.2</v>
       </c>
-      <c r="E36" s="50">
+      <c r="E36" s="61">
         <f>(D36*Estoque!E36)</f>
         <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.25" thickTop="1" thickBot="1"/>
     <row r="38" spans="1:5" ht="13.5" thickTop="1">
-      <c r="A38" s="33" t="s">
+      <c r="A38" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="41" t="s">
+      <c r="B38" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="43">
+      <c r="C38" s="30">
         <f>SUM(E6:E36)</f>
         <v>7140.5</v>
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="34"/>
-      <c r="B39" s="42" t="s">
+      <c r="A39" s="44"/>
+      <c r="B39" s="29" t="s">
         <v>84</v>
       </c>
       <c r="C39" s="7">
@@ -3563,7 +3542,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="13.5" thickBot="1">
-      <c r="A40" s="35"/>
+      <c r="A40" s="45"/>
       <c r="B40" s="4"/>
       <c r="C40" s="6"/>
     </row>
@@ -3607,14 +3586,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
@@ -3623,7 +3602,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>45</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -3636,21 +3615,21 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A2" s="36"/>
+      <c r="A2" s="46"/>
       <c r="B2" s="19"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" ht="13.5" thickTop="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="39"/>
+      <c r="B3" s="47" t="s">
         <v>46</v>
       </c>
       <c r="C3" s="3"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" ht="13.5" thickBot="1">
-      <c r="A4" s="29"/>
-      <c r="B4" s="38"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="20">
         <v>0.45</v>
       </c>
@@ -3660,15 +3639,15 @@
       <c r="G4" s="17"/>
     </row>
     <row r="5" spans="1:7" ht="13.5" thickTop="1">
-      <c r="A5" s="29"/>
+      <c r="A5" s="39"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="29"/>
+      <c r="A6" s="39"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="29"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -3689,7 +3668,7 @@
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="29"/>
+      <c r="A8" s="39"/>
       <c r="B8" s="10">
         <v>39448</v>
       </c>
@@ -3713,7 +3692,7 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="29"/>
+      <c r="A9" s="39"/>
       <c r="B9" s="10">
         <v>39448</v>
       </c>
@@ -3737,7 +3716,7 @@
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="29"/>
+      <c r="A10" s="39"/>
       <c r="B10" s="10">
         <v>39448</v>
       </c>
@@ -3761,7 +3740,7 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="29"/>
+      <c r="A11" s="39"/>
       <c r="B11" s="10">
         <v>39448</v>
       </c>
@@ -3785,7 +3764,7 @@
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="29"/>
+      <c r="A12" s="39"/>
       <c r="B12" s="10">
         <v>39448</v>
       </c>
@@ -3809,7 +3788,7 @@
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="29"/>
+      <c r="A13" s="39"/>
       <c r="B13" s="10">
         <v>39448</v>
       </c>
@@ -3833,7 +3812,7 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="29"/>
+      <c r="A14" s="39"/>
       <c r="B14" s="10">
         <v>39448</v>
       </c>
@@ -3857,7 +3836,7 @@
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="29"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="10">
         <v>39448</v>
       </c>
@@ -3881,7 +3860,7 @@
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="29"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="10">
         <v>39448</v>
       </c>
@@ -3905,7 +3884,7 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="29"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="10">
         <v>39448</v>
       </c>
@@ -3929,7 +3908,7 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="29"/>
+      <c r="A18" s="39"/>
       <c r="B18" s="10">
         <v>39448</v>
       </c>
@@ -3953,7 +3932,7 @@
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="29"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="10">
         <v>39448</v>
       </c>
@@ -3977,7 +3956,7 @@
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="29"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="10">
         <v>39448</v>
       </c>
@@ -4001,7 +3980,7 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="29"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="10">
         <v>39448</v>
       </c>
@@ -4025,7 +4004,7 @@
       </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="29"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="10">
         <v>39448</v>
       </c>
@@ -4049,7 +4028,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="29"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="10">
         <v>39448</v>
       </c>
@@ -4073,7 +4052,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="29"/>
+      <c r="A24" s="39"/>
       <c r="B24" s="10">
         <v>39448</v>
       </c>
@@ -4097,7 +4076,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="29"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="10">
         <v>39448</v>
       </c>
@@ -4121,7 +4100,7 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="29"/>
+      <c r="A26" s="39"/>
       <c r="B26" s="10">
         <v>39448</v>
       </c>
@@ -4145,7 +4124,7 @@
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="29"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="10">
         <v>39448</v>
       </c>
@@ -4169,7 +4148,7 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="29"/>
+      <c r="A28" s="39"/>
       <c r="B28" s="10">
         <v>39448</v>
       </c>
@@ -4193,7 +4172,7 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="29"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="10">
         <v>39448</v>
       </c>
@@ -4217,7 +4196,7 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="29"/>
+      <c r="A30" s="39"/>
       <c r="B30" s="10">
         <v>39448</v>
       </c>
@@ -4241,7 +4220,7 @@
       </c>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="29"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="10">
         <v>39448</v>
       </c>
@@ -4265,7 +4244,7 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="29"/>
+      <c r="A32" s="39"/>
       <c r="B32" s="10">
         <v>39448</v>
       </c>
@@ -4289,7 +4268,7 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="29"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="10">
         <v>39448</v>
       </c>
@@ -4313,7 +4292,7 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="29"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="10">
         <v>39448</v>
       </c>
@@ -4337,7 +4316,7 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="29"/>
+      <c r="A35" s="39"/>
       <c r="B35" s="10">
         <v>39448</v>
       </c>
@@ -4361,7 +4340,7 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="29"/>
+      <c r="A36" s="39"/>
       <c r="B36" s="10">
         <v>39448</v>
       </c>
@@ -4385,7 +4364,7 @@
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="29"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="10">
         <v>39448</v>
       </c>
@@ -4409,39 +4388,39 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="13.5" thickBot="1">
-      <c r="A38" s="30"/>
-      <c r="B38" s="46">
-        <v>39448</v>
-      </c>
-      <c r="C38" s="47" t="s">
+      <c r="A38" s="60"/>
+      <c r="B38" s="34">
+        <v>39448</v>
+      </c>
+      <c r="C38" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="D38" s="47">
+      <c r="D38" s="57">
         <v>35</v>
       </c>
-      <c r="E38" s="18">
+      <c r="E38" s="58">
         <f>'Valores Gastos'!D36+'Valores Gastos'!D36*($C$4)</f>
         <v>0.29000000000000004</v>
       </c>
-      <c r="F38" s="49">
+      <c r="F38" s="58">
         <f t="shared" si="0"/>
         <v>10.150000000000002</v>
       </c>
-      <c r="G38" s="50">
+      <c r="G38" s="59">
         <f>F38-'Valores Gastos'!E36</f>
         <v>0.15000000000000213</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.25" thickTop="1" thickBot="1"/>
     <row r="40" spans="1:7" ht="13.5" thickTop="1">
-      <c r="A40" s="33" t="s">
+      <c r="A40" s="43" t="s">
         <v>50</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="43"/>
+      <c r="C40" s="30"/>
     </row>
     <row r="41" spans="1:7" ht="13.5" thickBot="1">
-      <c r="A41" s="35"/>
+      <c r="A41" s="45"/>
       <c r="B41" s="4"/>
       <c r="C41" s="8">
         <f>SUM(F8:F38)</f>
@@ -4449,14 +4428,14 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="13.5" thickTop="1">
-      <c r="A42" s="33" t="s">
+      <c r="A42" s="43" t="s">
         <v>47</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="9"/>
     </row>
     <row r="43" spans="1:7" ht="13.5" thickBot="1">
-      <c r="A43" s="35"/>
+      <c r="A43" s="45"/>
       <c r="B43" s="4"/>
       <c r="C43" s="8">
         <f>('Vendas do Mes'!C41-'Valores Gastos'!C38)</f>
@@ -4529,18 +4508,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7.85546875" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -4549,7 +4528,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickTop="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="49" t="s">
         <v>78</v>
       </c>
       <c r="B1" s="13" t="s">
@@ -4560,18 +4539,18 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
-      <c r="J1" s="44"/>
-      <c r="O1" s="62"/>
+      <c r="J1" s="31"/>
+      <c r="O1" s="54"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="40"/>
+      <c r="A2" s="50"/>
       <c r="B2" s="14"/>
       <c r="G2" s="5"/>
-      <c r="J2" s="44"/>
-      <c r="O2" s="62"/>
+      <c r="J2" s="31"/>
+      <c r="O2" s="54"/>
     </row>
     <row r="3" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A3" s="40"/>
+      <c r="A3" s="50"/>
       <c r="B3" s="15" t="s">
         <v>34</v>
       </c>
@@ -4583,19 +4562,18 @@
       <c r="O3" s="17"/>
     </row>
     <row r="4" spans="1:15" ht="13.5" thickTop="1">
-      <c r="A4" s="40"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="61"/>
+      <c r="A4" s="50"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="37"/>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="40"/>
+      <c r="A5" s="50"/>
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -4614,10 +4592,10 @@
       <c r="G5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O5" s="62"/>
+      <c r="O5" s="54"/>
     </row>
     <row r="6" spans="1:15">
-      <c r="A6" s="40"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="10">
         <v>39477</v>
       </c>
@@ -4636,14 +4614,14 @@
         <f>(D6-E6)</f>
         <v>10</v>
       </c>
-      <c r="G6" s="54" t="str">
+      <c r="G6" s="33" t="str">
         <f>IF(F6=0,"20 UNIDADES","NÃO PRECISA COMPRAR!")</f>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O6" s="62"/>
+      <c r="O6" s="54"/>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7" s="40"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="10">
         <v>39477</v>
       </c>
@@ -4662,14 +4640,14 @@
         <f t="shared" ref="F7:F36" si="0">(D7-E7)</f>
         <v>20</v>
       </c>
-      <c r="G7" s="54" t="str">
+      <c r="G7" s="33" t="str">
         <f t="shared" ref="G7:G36" si="1">IF(F7=0,"20 UNIDADES","NÃO PRECISA COMPRAR!")</f>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O7" s="62"/>
+      <c r="O7" s="54"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8" s="40"/>
+      <c r="A8" s="50"/>
       <c r="B8" s="10">
         <v>39477</v>
       </c>
@@ -4688,14 +4666,15 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G8" s="54" t="str">
+      <c r="G8" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O8" s="62"/>
+      <c r="H8" s="29"/>
+      <c r="O8" s="54"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9" s="40"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="10">
         <v>39477</v>
       </c>
@@ -4714,14 +4693,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="54" t="str">
+      <c r="G9" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O9" s="62"/>
+      <c r="O9" s="54"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10" s="40"/>
+      <c r="A10" s="50"/>
       <c r="B10" s="10">
         <v>39477</v>
       </c>
@@ -4740,14 +4719,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="54" t="str">
+      <c r="G10" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O10" s="62"/>
+      <c r="O10" s="54"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11" s="40"/>
+      <c r="A11" s="50"/>
       <c r="B11" s="10">
         <v>39477</v>
       </c>
@@ -4766,14 +4745,14 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G11" s="54" t="str">
+      <c r="G11" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O11" s="62"/>
+      <c r="O11" s="54"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="A12" s="40"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="10">
         <v>39477</v>
       </c>
@@ -4792,14 +4771,14 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="G12" s="54" t="str">
+      <c r="G12" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O12" s="62"/>
+      <c r="O12" s="54"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="A13" s="40"/>
+      <c r="A13" s="50"/>
       <c r="B13" s="10">
         <v>39477</v>
       </c>
@@ -4818,14 +4797,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G13" s="54" t="str">
+      <c r="G13" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O13" s="62"/>
+      <c r="O13" s="54"/>
     </row>
     <row r="14" spans="1:15">
-      <c r="A14" s="40"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="10">
         <v>39477</v>
       </c>
@@ -4844,14 +4823,14 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G14" s="54" t="str">
+      <c r="G14" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O14" s="62"/>
+      <c r="O14" s="54"/>
     </row>
     <row r="15" spans="1:15">
-      <c r="A15" s="40"/>
+      <c r="A15" s="50"/>
       <c r="B15" s="10">
         <v>39477</v>
       </c>
@@ -4870,14 +4849,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G15" s="54" t="str">
+      <c r="G15" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O15" s="62"/>
+      <c r="O15" s="54"/>
     </row>
     <row r="16" spans="1:15">
-      <c r="A16" s="40"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="10">
         <v>39477</v>
       </c>
@@ -4896,14 +4875,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G16" s="54" t="str">
+      <c r="G16" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O16" s="62"/>
+      <c r="O16" s="54"/>
     </row>
     <row r="17" spans="1:15">
-      <c r="A17" s="40"/>
+      <c r="A17" s="50"/>
       <c r="B17" s="10">
         <v>39477</v>
       </c>
@@ -4922,15 +4901,15 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G17" s="54" t="str">
+      <c r="G17" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="L17" s="45"/>
-      <c r="O17" s="62"/>
+      <c r="L17" s="32"/>
+      <c r="O17" s="54"/>
     </row>
     <row r="18" spans="1:15">
-      <c r="A18" s="40"/>
+      <c r="A18" s="50"/>
       <c r="B18" s="10">
         <v>39477</v>
       </c>
@@ -4949,14 +4928,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G18" s="54" t="str">
+      <c r="G18" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O18" s="62"/>
+      <c r="O18" s="54"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="40"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="10">
         <v>39477</v>
       </c>
@@ -4975,14 +4954,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G19" s="54" t="str">
+      <c r="G19" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O19" s="62"/>
+      <c r="O19" s="54"/>
     </row>
     <row r="20" spans="1:15">
-      <c r="A20" s="40"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="10">
         <v>39477</v>
       </c>
@@ -5001,14 +4980,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="54" t="str">
+      <c r="G20" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O20" s="62"/>
+      <c r="O20" s="54"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="40"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="10">
         <v>39477</v>
       </c>
@@ -5027,14 +5006,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G21" s="54" t="str">
+      <c r="G21" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O21" s="62"/>
+      <c r="O21" s="54"/>
     </row>
     <row r="22" spans="1:15">
-      <c r="A22" s="40"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="10">
         <v>39477</v>
       </c>
@@ -5053,14 +5032,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G22" s="54" t="str">
+      <c r="G22" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O22" s="62"/>
+      <c r="O22" s="54"/>
     </row>
     <row r="23" spans="1:15">
-      <c r="A23" s="40"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="10">
         <v>39477</v>
       </c>
@@ -5079,14 +5058,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G23" s="54" t="str">
+      <c r="G23" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O23" s="62"/>
+      <c r="O23" s="54"/>
     </row>
     <row r="24" spans="1:15">
-      <c r="A24" s="40"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="10">
         <v>39477</v>
       </c>
@@ -5105,14 +5084,14 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G24" s="54" t="str">
+      <c r="G24" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O24" s="62"/>
+      <c r="O24" s="54"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="A25" s="40"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="10">
         <v>39477</v>
       </c>
@@ -5131,14 +5110,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G25" s="54" t="str">
+      <c r="G25" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O25" s="62"/>
+      <c r="O25" s="54"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="A26" s="40"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="10">
         <v>39477</v>
       </c>
@@ -5157,14 +5136,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G26" s="54" t="str">
+      <c r="G26" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O26" s="62"/>
+      <c r="O26" s="54"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="A27" s="40"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="10">
         <v>39477</v>
       </c>
@@ -5183,14 +5162,14 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G27" s="54" t="str">
+      <c r="G27" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O27" s="62"/>
+      <c r="O27" s="54"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="A28" s="40"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="10">
         <v>39477</v>
       </c>
@@ -5209,14 +5188,14 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G28" s="54" t="str">
+      <c r="G28" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O28" s="62"/>
+      <c r="O28" s="54"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="A29" s="40"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="10">
         <v>39477</v>
       </c>
@@ -5235,21 +5214,14 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G29" s="54" t="str">
+      <c r="G29" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="I29" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="J29" s="44">
-        <f>'Valores Gastos'!C38</f>
-        <v>7140.5</v>
-      </c>
-      <c r="O29" s="62"/>
+      <c r="O29" s="54"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="A30" s="40"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="10">
         <v>39477</v>
       </c>
@@ -5268,21 +5240,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G30" s="54" t="str">
+      <c r="G30" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="I30" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="J30" s="44">
-        <f>'Vendas do Mes'!C41</f>
-        <v>9694.6999999999989</v>
-      </c>
-      <c r="O30" s="62"/>
+      <c r="O30" s="54"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="40"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="10">
         <v>39477</v>
       </c>
@@ -5301,14 +5266,14 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G31" s="54" t="str">
+      <c r="G31" s="33" t="str">
         <f t="shared" si="1"/>
         <v>20 UNIDADES</v>
       </c>
-      <c r="O31" s="62"/>
+      <c r="O31" s="54"/>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="40"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="10">
         <v>39477</v>
       </c>
@@ -5327,14 +5292,14 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G32" s="54" t="str">
+      <c r="G32" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O32" s="62"/>
+      <c r="O32" s="54"/>
     </row>
     <row r="33" spans="1:15">
-      <c r="A33" s="40"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="10">
         <v>39477</v>
       </c>
@@ -5353,14 +5318,14 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="G33" s="54" t="str">
+      <c r="G33" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O33" s="62"/>
+      <c r="O33" s="54"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="A34" s="40"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="10">
         <v>39477</v>
       </c>
@@ -5379,14 +5344,21 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G34" s="54" t="str">
+      <c r="G34" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O34" s="62"/>
+      <c r="I34" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="J34" s="31">
+        <f>'Valores Gastos'!C38</f>
+        <v>7140.5</v>
+      </c>
+      <c r="O34" s="54"/>
     </row>
     <row r="35" spans="1:15">
-      <c r="A35" s="40"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="10">
         <v>39477</v>
       </c>
@@ -5405,15 +5377,22 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="G35" s="54" t="str">
+      <c r="G35" s="33" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O35" s="62"/>
+      <c r="I35" s="56" t="s">
+        <v>86</v>
+      </c>
+      <c r="J35" s="31">
+        <f>'Vendas do Mes'!C41</f>
+        <v>9694.6999999999989</v>
+      </c>
+      <c r="O35" s="54"/>
     </row>
     <row r="36" spans="1:15" ht="13.5" thickBot="1">
-      <c r="A36" s="56"/>
-      <c r="B36" s="57">
+      <c r="A36" s="51"/>
+      <c r="B36" s="34">
         <v>39477</v>
       </c>
       <c r="C36" s="4" t="s">
@@ -5431,11 +5410,18 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G36" s="55" t="str">
+      <c r="G36" s="52" t="str">
         <f t="shared" si="1"/>
         <v>NÃO PRECISA COMPRAR!</v>
       </c>
-      <c r="O36" s="62"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="6"/>
     </row>
     <row r="37" spans="1:15" ht="13.5" thickTop="1"/>
     <row r="38" spans="1:15">

</xml_diff>